<commit_message>
Update uni and bivariate analyses.
</commit_message>
<xml_diff>
--- a/Project 1-Python Foundations/foodhub_order.xlsx
+++ b/Project 1-Python Foundations/foodhub_order.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamessomerville/git/PGP-AI-ML-BA-UTA-JS/Project 1-Python Foundations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DF40146B-36F1-544B-9813-2F93F7E9C367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D041E9-6586-F14E-BB67-65D027610A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="700" windowWidth="26740" windowHeight="15160"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foodhub_order" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6439" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6447" uniqueCount="212">
   <si>
     <t>order_id</t>
   </si>
@@ -633,11 +647,35 @@
   <si>
     <t>'wichcraft</t>
   </si>
+  <si>
+    <t>Promote weekday deliveries</t>
+  </si>
+  <si>
+    <t>Promote alternative cuisines/restaurants</t>
+  </si>
+  <si>
+    <t>Encourage multiple person orders to increase revenue per order</t>
+  </si>
+  <si>
+    <t>Rewards program to incentivize repeat customers as most are single time customers.</t>
+  </si>
+  <si>
+    <t>Investigate cause and mitigations for long orders (over an hour)</t>
+  </si>
+  <si>
+    <t>Investigate cause and mitigations for deliveries being ~27% slower during weekdays</t>
+  </si>
+  <si>
+    <t>Average reviews or ratings are very high for the service. However, nearly 40% of customers don't provide a rating. To ensure consistent high quality, find ways to encourage customers to provide ratings.</t>
+  </si>
+  <si>
+    <t>Some cuisine types are more costly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1115,8 +1153,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1471,10 +1511,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1899"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -56565,4 +56605,71 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0085E887-AEB6-7B45-988E-3238F3F6813B}">
+  <dimension ref="B2:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O10" s="1">
+        <f>6/22</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <f>736/1899</f>
+        <v>0.3875724065297525</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final updates for submission
</commit_message>
<xml_diff>
--- a/Project 1-Python Foundations/foodhub_order.xlsx
+++ b/Project 1-Python Foundations/foodhub_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamessomerville/git/PGP-AI-ML-BA-UTA-JS/Project 1-Python Foundations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D041E9-6586-F14E-BB67-65D027610A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FFBC10-6391-AC46-82EA-C4F2A482E5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foodhub_order" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6447" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6453" uniqueCount="214">
   <si>
     <t>order_id</t>
   </si>
@@ -666,10 +666,16 @@
     <t>Investigate cause and mitigations for deliveries being ~27% slower during weekdays</t>
   </si>
   <si>
-    <t>Average reviews or ratings are very high for the service. However, nearly 40% of customers don't provide a rating. To ensure consistent high quality, find ways to encourage customers to provide ratings.</t>
+    <t>Some cuisine types are more costly</t>
   </si>
   <si>
-    <t>Some cuisine types are more costly</t>
+    <t>Average reviews or ratings are very high for the service.</t>
+  </si>
+  <si>
+    <t>Nearly 40% of customers don't provide a rating. To ensure consistent high quality, find ways to encourage customers to provide ratings.</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1153,10 +1159,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -56609,61 +56614,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0085E887-AEB6-7B45-988E-3238F3F6813B}">
-  <dimension ref="B2:O11"/>
+  <dimension ref="A2:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>213</v>
+      </c>
       <c r="B6" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
       <c r="B7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
       <c r="O10" s="1">
         <f>6/22</f>
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O11">
         <f>736/1899</f>
         <v>0.3875724065297525</v>
@@ -56671,5 +56694,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>